<commit_message>
updates to CGINS-DOSTAJ-00352 (legacy_uid N00580)
CGINS-DOSTAJ-00352 (legacy_uid N00580) was previously assigned an
incorrect serial number (351). The S/N was updated (correct S/N 352) in
sensor_bulk_load and the cal sheet names in a previous commit. The MIO
provided corrected calibration coefficients for this instrument

-updated the cal sheet with corrected values (and archived cal sheets)
-removed duplicated cal sheets
-changed cal sheet name to contain the date of calibration rather than
date of first deployment
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00002.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00002.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CE_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgarzio/Documents/repo/lgarzio/ooi-integration-fork/asset-management/ARCHIVE/deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="579"/>
+    <workbookView xWindow="9580" yWindow="11420" windowWidth="25600" windowHeight="16060" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -26,8 +26,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$I$51</definedName>
     <definedName name="Workbook1" localSheetId="1">Asset_Cal_Info!$H$5:$H$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="114">
   <si>
     <t>Ref Des</t>
   </si>
@@ -400,6 +403,9 @@
   </si>
   <si>
     <t>Sensor OOIBARCODE</t>
+  </si>
+  <si>
+    <t>corrected cal values: [0.00283856, 0.000119430, 2.41799e-06, 231.190, -0.328248, -55.9998, 4.55859]</t>
   </si>
 </sst>
 </file>
@@ -2246,28 +2252,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -2349,13 +2355,13 @@
         <v>-124.09566666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
@@ -2364,7 +2370,7 @@
         <v>44.664153333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -2373,73 +2379,73 @@
         <v>-124.09566666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="4:7" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
@@ -2448,38 +2454,33 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="17" style="47" customWidth="1"/>
-    <col min="7" max="7" width="32.77734375" customWidth="1"/>
-    <col min="8" max="8" width="37.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.83203125" customWidth="1"/>
+    <col min="8" max="8" width="37.5" style="3" customWidth="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -2519,7 +2520,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>104</v>
       </c>
       <c r="F3" s="44">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>7</v>
@@ -2548,7 +2549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>91</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>104</v>
       </c>
       <c r="F4" s="44">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>8</v>
@@ -2577,7 +2578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>91</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>104</v>
       </c>
       <c r="F5" s="44">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>6</v>
@@ -2602,7 +2603,9 @@
       <c r="H5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="31" t="s">
+        <v>113</v>
+      </c>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -2610,7 +2613,7 @@
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
     </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>91</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>104</v>
       </c>
       <c r="F6" s="44">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>62</v>
@@ -2639,7 +2642,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="21"/>
@@ -2650,7 +2653,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>92</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>92</v>
       </c>
@@ -2706,7 +2709,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>92</v>
       </c>
@@ -2733,7 +2736,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>92</v>
       </c>
@@ -2760,7 +2763,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>92</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>92</v>
       </c>
@@ -2814,7 +2817,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>92</v>
       </c>
@@ -2841,7 +2844,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>92</v>
       </c>
@@ -2868,7 +2871,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="21"/>
@@ -2879,7 +2882,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>93</v>
       </c>
@@ -2908,7 +2911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>93</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="21"/>
@@ -2948,7 +2951,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>94</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>94</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>94</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>94</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>94</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>94</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>94</v>
       </c>
@@ -3151,7 +3154,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="21"/>
@@ -3162,7 +3165,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>95</v>
       </c>
@@ -3189,7 +3192,7 @@
       </c>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>95</v>
       </c>
@@ -3216,7 +3219,7 @@
       </c>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>95</v>
       </c>
@@ -3243,7 +3246,7 @@
       </c>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="21"/>
@@ -3254,7 +3257,7 @@
       <c r="H31" s="19"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>96</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>96</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>96</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>96</v>
       </c>
@@ -3370,7 +3373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>96</v>
       </c>
@@ -3399,7 +3402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>96</v>
       </c>
@@ -3428,7 +3431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>96</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>96</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>96</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>96</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="21"/>
@@ -3555,7 +3558,7 @@
       <c r="H42" s="19"/>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>97</v>
       </c>
@@ -3584,7 +3587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
         <v>97</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="21"/>
@@ -3624,7 +3627,7 @@
       <c r="H45" s="19"/>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>98</v>
       </c>
@@ -3651,7 +3654,7 @@
       </c>
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>98</v>
       </c>
@@ -3678,7 +3681,7 @@
       </c>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>98</v>
       </c>
@@ -3705,7 +3708,7 @@
       </c>
       <c r="I48" s="14"/>
     </row>
-    <row r="49" spans="1:9" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A49" s="27"/>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
@@ -3716,7 +3719,7 @@
       <c r="H49" s="28"/>
       <c r="I49" s="27"/>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="29" t="s">
         <v>99</v>
       </c>
@@ -3739,27 +3742,22 @@
       <c r="H50" s="30"/>
       <c r="I50" s="14"/>
     </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F51" s="47"/>
     </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F52" s="47"/>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F53" s="47"/>
     </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F54" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="3" scale="89" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3771,9 +3769,9 @@
       <selection sqref="A1:AH86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>-2.7306E-2</v>
       </c>
@@ -3877,7 +3875,7 @@
         <v>2.2003000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-2.1257999999999999E-2</v>
       </c>
@@ -3981,7 +3979,7 @@
         <v>1.6747000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1.2599000000000001E-2</v>
       </c>
@@ -4085,7 +4083,7 @@
         <v>1.111E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-4.3949999999999996E-3</v>
       </c>
@@ -4189,7 +4187,7 @@
         <v>3.9740000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.9880000000000002E-3</v>
       </c>
@@ -4293,7 +4291,7 @@
         <v>-3.1E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7.7140000000000004E-3</v>
       </c>
@@ -4397,7 +4395,7 @@
         <v>-3.039E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.038E-2</v>
       </c>
@@ -4501,7 +4499,7 @@
         <v>-4.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.0441000000000001E-2</v>
       </c>
@@ -4605,7 +4603,7 @@
         <v>-5.3030000000000004E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9.8150000000000008E-3</v>
       </c>
@@ -4709,7 +4707,7 @@
         <v>-5.378E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9.7280000000000005E-3</v>
       </c>
@@ -4813,7 +4811,7 @@
         <v>-5.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9.1170000000000001E-3</v>
       </c>
@@ -4917,7 +4915,7 @@
         <v>-5.104E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9.0360000000000006E-3</v>
       </c>
@@ -5021,7 +5019,7 @@
         <v>-4.7270000000000003E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8.0409999999999995E-3</v>
       </c>
@@ -5125,7 +5123,7 @@
         <v>-4.3819999999999996E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8.1829999999999993E-3</v>
       </c>
@@ -5229,7 +5227,7 @@
         <v>-4.5630000000000002E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8.2159999999999993E-3</v>
       </c>
@@ -5333,7 +5331,7 @@
         <v>-4.4270000000000004E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7.6169999999999996E-3</v>
       </c>
@@ -5437,7 +5435,7 @@
         <v>-4.1739999999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6.7520000000000002E-3</v>
       </c>
@@ -5541,7 +5539,7 @@
         <v>-4.1269999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7.0699999999999999E-3</v>
       </c>
@@ -5645,7 +5643,7 @@
         <v>-4.1380000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6.8310000000000003E-3</v>
       </c>
@@ -5749,7 +5747,7 @@
         <v>-4.1419999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6.4079999999999996E-3</v>
       </c>
@@ -5853,7 +5851,7 @@
         <v>-4.2430000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6.4419999999999998E-3</v>
       </c>
@@ -5957,7 +5955,7 @@
         <v>-4.2009999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6.2509999999999996E-3</v>
       </c>
@@ -6061,7 +6059,7 @@
         <v>-4.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6.1939999999999999E-3</v>
       </c>
@@ -6165,7 +6163,7 @@
         <v>-3.9050000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5.6759999999999996E-3</v>
       </c>
@@ -6269,7 +6267,7 @@
         <v>-3.9870000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5.3439999999999998E-3</v>
       </c>
@@ -6373,7 +6371,7 @@
         <v>-3.7260000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5.2090000000000001E-3</v>
       </c>
@@ -6477,7 +6475,7 @@
         <v>-3.5729999999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4.9170000000000004E-3</v>
       </c>
@@ -6581,7 +6579,7 @@
         <v>-3.578E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4.7239999999999999E-3</v>
       </c>
@@ -6685,7 +6683,7 @@
         <v>-3.392E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4.0660000000000002E-3</v>
       </c>
@@ -6789,7 +6787,7 @@
         <v>-3.2490000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4.2430000000000002E-3</v>
       </c>
@@ -6893,7 +6891,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3.777E-3</v>
       </c>
@@ -6997,7 +6995,7 @@
         <v>-3.0130000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3.607E-3</v>
       </c>
@@ -7101,7 +7099,7 @@
         <v>-2.7659999999999998E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3.2729999999999999E-3</v>
       </c>
@@ -7205,7 +7203,7 @@
         <v>-2.5219999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3.0950000000000001E-3</v>
       </c>
@@ -7309,7 +7307,7 @@
         <v>-2.2269999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3.0699999999999998E-3</v>
       </c>
@@ -7413,7 +7411,7 @@
         <v>-1.8309999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3.0349999999999999E-3</v>
       </c>
@@ -7517,7 +7515,7 @@
         <v>-1.588E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3.2399999999999998E-3</v>
       </c>
@@ -7621,7 +7619,7 @@
         <v>-1.4289999999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3.1510000000000002E-3</v>
       </c>
@@ -7725,7 +7723,7 @@
         <v>-1.129E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3.0019999999999999E-3</v>
       </c>
@@ -7829,7 +7827,7 @@
         <v>-1.0009999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2.911E-3</v>
       </c>
@@ -7933,7 +7931,7 @@
         <v>-9.6299999999999999E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2.9169999999999999E-3</v>
       </c>
@@ -8037,7 +8035,7 @@
         <v>-9.0200000000000002E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2.4870000000000001E-3</v>
       </c>
@@ -8141,7 +8139,7 @@
         <v>-8.8800000000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2.565E-3</v>
       </c>
@@ -8245,7 +8243,7 @@
         <v>-8.7500000000000002E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2.1519999999999998E-3</v>
       </c>
@@ -8349,7 +8347,7 @@
         <v>-9.0399999999999996E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1.918E-3</v>
       </c>
@@ -8453,7 +8451,7 @@
         <v>1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2.2130000000000001E-3</v>
       </c>
@@ -8557,7 +8555,7 @@
         <v>1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2.3509999999999998E-3</v>
       </c>
@@ -8661,7 +8659,7 @@
         <v>-8.2999999999999998E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2.6870000000000002E-3</v>
       </c>
@@ -8765,7 +8763,7 @@
         <v>-1.3200000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2.7929999999999999E-3</v>
       </c>
@@ -8869,7 +8867,7 @@
         <v>-3.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2.7260000000000001E-3</v>
       </c>
@@ -8973,7 +8971,7 @@
         <v>-4.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2.859E-3</v>
       </c>
@@ -9077,7 +9075,7 @@
         <v>-4.6200000000000001E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2.8110000000000001E-3</v>
       </c>
@@ -9181,7 +9179,7 @@
         <v>-6.5300000000000004E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2.5959999999999998E-3</v>
       </c>
@@ -9285,7 +9283,7 @@
         <v>-6.4199999999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2.3879999999999999E-3</v>
       </c>
@@ -9389,7 +9387,7 @@
         <v>-6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2.1250000000000002E-3</v>
       </c>
@@ -9493,7 +9491,7 @@
         <v>-7.5299999999999998E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1.838E-3</v>
       </c>
@@ -9597,7 +9595,7 @@
         <v>-7.6499999999999995E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1.5709999999999999E-3</v>
       </c>
@@ -9701,7 +9699,7 @@
         <v>-8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1.358E-3</v>
       </c>
@@ -9805,7 +9803,7 @@
         <v>-8.6399999999999997E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1.088E-3</v>
       </c>
@@ -9909,7 +9907,7 @@
         <v>-9.5699999999999995E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8.8999999999999995E-4</v>
       </c>
@@ -10013,7 +10011,7 @@
         <v>-9.4300000000000004E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>4.75E-4</v>
       </c>
@@ -10117,7 +10115,7 @@
         <v>-1.0709999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2.5300000000000002E-4</v>
       </c>
@@ -10221,7 +10219,7 @@
         <v>-1.163E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2.23E-4</v>
       </c>
@@ -10325,7 +10323,7 @@
         <v>-1.232E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-2.13E-4</v>
       </c>
@@ -10429,7 +10427,7 @@
         <v>-1.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-3.5300000000000002E-4</v>
       </c>
@@ -10533,7 +10531,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-6.9099999999999999E-4</v>
       </c>
@@ -10637,7 +10635,7 @@
         <v>-1.371E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-6.6200000000000005E-4</v>
       </c>
@@ -10741,7 +10739,7 @@
         <v>-1.4250000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-8.6600000000000002E-4</v>
       </c>
@@ -10845,7 +10843,7 @@
         <v>-1.436E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-9.8299999999999993E-4</v>
       </c>
@@ -10949,7 +10947,7 @@
         <v>-1.5219999999999999E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-1.134E-3</v>
       </c>
@@ -11053,7 +11051,7 @@
         <v>-1.578E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-1.106E-3</v>
       </c>
@@ -11157,7 +11155,7 @@
         <v>-1.518E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-1.542E-3</v>
       </c>
@@ -11261,7 +11259,7 @@
         <v>-1.5120000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>-1.658E-3</v>
       </c>
@@ -11365,7 +11363,7 @@
         <v>-1.4729999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>-1.7930000000000001E-3</v>
       </c>
@@ -11469,7 +11467,7 @@
         <v>-1.3110000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>-1.9610000000000001E-3</v>
       </c>
@@ -11573,7 +11571,7 @@
         <v>-1.0709999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>-1.92E-3</v>
       </c>
@@ -11677,7 +11675,7 @@
         <v>-8.12E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>-2.1649999999999998E-3</v>
       </c>
@@ -11781,7 +11779,7 @@
         <v>-5.9800000000000001E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>-2.274E-3</v>
       </c>
@@ -11885,7 +11883,7 @@
         <v>-3.3300000000000002E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>-2.4229999999999998E-3</v>
       </c>
@@ -11989,7 +11987,7 @@
         <v>-2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>-2.5240000000000002E-3</v>
       </c>
@@ -12093,7 +12091,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>-2.5490000000000001E-3</v>
       </c>
@@ -12197,7 +12195,7 @@
         <v>2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>-2.5799999999999998E-3</v>
       </c>
@@ -12301,7 +12299,7 @@
         <v>4.5600000000000003E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>-2.421E-3</v>
       </c>
@@ -12405,7 +12403,7 @@
         <v>4.3100000000000001E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>-2.4420000000000002E-3</v>
       </c>
@@ -12509,7 +12507,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>-2.117E-3</v>
       </c>
@@ -12613,7 +12611,7 @@
         <v>4.8200000000000001E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>-2.3029999999999999E-3</v>
       </c>
@@ -12719,11 +12717,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12735,9 +12728,9 @@
       <selection sqref="A1:AH86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2.818E-2</v>
       </c>
@@ -12841,7 +12834,7 @@
         <v>-1.3003000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.9113999999999999E-2</v>
       </c>
@@ -12945,7 +12938,7 @@
         <v>-1.0573000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.0387E-2</v>
       </c>
@@ -13049,7 +13042,7 @@
         <v>-9.0050000000000009E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6.8069999999999997E-3</v>
       </c>
@@ -13153,7 +13146,7 @@
         <v>-8.1989999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5.4920000000000004E-3</v>
       </c>
@@ -13257,7 +13250,7 @@
         <v>-6.4209999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3.483E-3</v>
       </c>
@@ -13361,7 +13354,7 @@
         <v>-5.2810000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2.4060000000000002E-3</v>
       </c>
@@ -13465,7 +13458,7 @@
         <v>-4.2729999999999999E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.4300000000000001E-3</v>
       </c>
@@ -13569,7 +13562,7 @@
         <v>-3.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-1.129E-3</v>
       </c>
@@ -13673,7 +13666,7 @@
         <v>-2.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-1.812E-3</v>
       </c>
@@ -13777,7 +13770,7 @@
         <v>-1.8680000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-2.7070000000000002E-3</v>
       </c>
@@ -13881,7 +13874,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-4.6169999999999996E-3</v>
       </c>
@@ -13985,7 +13978,7 @@
         <v>-7.1100000000000004E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-4.8739999999999999E-3</v>
       </c>
@@ -14089,7 +14082,7 @@
         <v>-5.8999999999999998E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-5.3109999999999997E-3</v>
       </c>
@@ -14193,7 +14186,7 @@
         <v>6.6600000000000003E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-6.7479999999999997E-3</v>
       </c>
@@ -14297,7 +14290,7 @@
         <v>9.2900000000000003E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-6.149E-3</v>
       </c>
@@ -14401,7 +14394,7 @@
         <v>1.4610000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-6.437E-3</v>
       </c>
@@ -14505,7 +14498,7 @@
         <v>1.7589999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-7.2789999999999999E-3</v>
       </c>
@@ -14609,7 +14602,7 @@
         <v>2.1549999999999998E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-7.6649999999999999E-3</v>
       </c>
@@ -14713,7 +14706,7 @@
         <v>2.1870000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-8.8280000000000008E-3</v>
       </c>
@@ -14817,7 +14810,7 @@
         <v>2.5990000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-9.3799999999999994E-3</v>
       </c>
@@ -14921,7 +14914,7 @@
         <v>2.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-9.2580000000000006E-3</v>
       </c>
@@ -15025,7 +15018,7 @@
         <v>2.8349999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-1.0026E-2</v>
       </c>
@@ -15129,7 +15122,7 @@
         <v>2.7989999999999998E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-1.0159E-2</v>
       </c>
@@ -15233,7 +15226,7 @@
         <v>2.8739999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-9.9780000000000008E-3</v>
       </c>
@@ -15337,7 +15330,7 @@
         <v>2.8479999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-1.0371E-2</v>
       </c>
@@ -15441,7 +15434,7 @@
         <v>2.7680000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-1.0656000000000001E-2</v>
       </c>
@@ -15545,7 +15538,7 @@
         <v>2.8119999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-1.0642E-2</v>
       </c>
@@ -15649,7 +15642,7 @@
         <v>2.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-1.0969E-2</v>
       </c>
@@ -15753,7 +15746,7 @@
         <v>2.7669999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-1.1292E-2</v>
       </c>
@@ -15857,7 +15850,7 @@
         <v>2.771E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-1.0963000000000001E-2</v>
       </c>
@@ -15961,7 +15954,7 @@
         <v>2.5690000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-1.1731999999999999E-2</v>
       </c>
@@ -16065,7 +16058,7 @@
         <v>2.506E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-1.1818E-2</v>
       </c>
@@ -16169,7 +16162,7 @@
         <v>2.369E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-1.2111E-2</v>
       </c>
@@ -16273,7 +16266,7 @@
         <v>2.212E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-1.2655E-2</v>
       </c>
@@ -16377,7 +16370,7 @@
         <v>2.1180000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-1.2838E-2</v>
       </c>
@@ -16481,7 +16474,7 @@
         <v>2.0839999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-1.2978999999999999E-2</v>
       </c>
@@ -16585,7 +16578,7 @@
         <v>2.0790000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-1.304E-2</v>
       </c>
@@ -16689,7 +16682,7 @@
         <v>2.0609999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-1.2704999999999999E-2</v>
       </c>
@@ -16793,7 +16786,7 @@
         <v>2.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-1.2663000000000001E-2</v>
       </c>
@@ -16897,7 +16890,7 @@
         <v>2.0089999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>-1.2364999999999999E-2</v>
       </c>
@@ -17001,7 +16994,7 @@
         <v>2.032E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-1.2322E-2</v>
       </c>
@@ -17105,7 +17098,7 @@
         <v>2.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-1.1955E-2</v>
       </c>
@@ -17209,7 +17202,7 @@
         <v>2.1069999999999999E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-1.2149E-2</v>
       </c>
@@ -17313,7 +17306,7 @@
         <v>2.0170000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-7.4850000000000003E-3</v>
       </c>
@@ -17417,7 +17410,7 @@
         <v>8.8599999999999996E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-7.2389999999999998E-3</v>
       </c>
@@ -17521,7 +17514,7 @@
         <v>7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-7.123E-3</v>
       </c>
@@ -17625,7 +17618,7 @@
         <v>6.3500000000000004E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-6.8180000000000003E-3</v>
       </c>
@@ -17729,7 +17722,7 @@
         <v>5.2599999999999999E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-6.8339999999999998E-3</v>
       </c>
@@ -17833,7 +17826,7 @@
         <v>5.1099999999999995E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-6.881E-3</v>
       </c>
@@ -17937,7 +17930,7 @@
         <v>6.2399999999999999E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-6.9410000000000001E-3</v>
       </c>
@@ -18041,7 +18034,7 @@
         <v>6.7599999999999995E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-7.0809999999999996E-3</v>
       </c>
@@ -18145,7 +18138,7 @@
         <v>8.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-7.2399999999999999E-3</v>
       </c>
@@ -18249,7 +18242,7 @@
         <v>9.2699999999999998E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-7.4229999999999999E-3</v>
       </c>
@@ -18353,7 +18346,7 @@
         <v>1.114E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-7.6220000000000003E-3</v>
       </c>
@@ -18457,7 +18450,7 @@
         <v>1.3140000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-7.8150000000000008E-3</v>
       </c>
@@ -18561,7 +18554,7 @@
         <v>1.4549999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-8.0059999999999992E-3</v>
       </c>
@@ -18665,7 +18658,7 @@
         <v>1.5709999999999999E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-8.1650000000000004E-3</v>
       </c>
@@ -18769,7 +18762,7 @@
         <v>1.604E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-8.2880000000000002E-3</v>
       </c>
@@ -18873,7 +18866,7 @@
         <v>1.784E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-8.456E-3</v>
       </c>
@@ -18977,7 +18970,7 @@
         <v>1.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-8.6499999999999997E-3</v>
       </c>
@@ -19081,7 +19074,7 @@
         <v>1.897E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-8.6359999999999996E-3</v>
       </c>
@@ -19185,7 +19178,7 @@
         <v>1.7960000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-8.2819999999999994E-3</v>
       </c>
@@ -19289,7 +19282,7 @@
         <v>1.9239999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-8.7810000000000006E-3</v>
       </c>
@@ -19393,7 +19386,7 @@
         <v>1.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-8.659E-3</v>
       </c>
@@ -19497,7 +19490,7 @@
         <v>1.9350000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-8.5939999999999992E-3</v>
       </c>
@@ -19601,7 +19594,7 @@
         <v>1.9689999999999998E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-8.9849999999999999E-3</v>
       </c>
@@ -19705,7 +19698,7 @@
         <v>1.884E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-8.744E-3</v>
       </c>
@@ -19809,7 +19802,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-8.9210000000000001E-3</v>
       </c>
@@ -19913,7 +19906,7 @@
         <v>1.913E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-8.9890000000000005E-3</v>
       </c>
@@ -20017,7 +20010,7 @@
         <v>1.8760000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-9.1999999999999998E-3</v>
       </c>
@@ -20121,7 +20114,7 @@
         <v>1.8259999999999999E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-9.391E-3</v>
       </c>
@@ -20225,7 +20218,7 @@
         <v>1.7700000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>-9.4769999999999993E-3</v>
       </c>
@@ -20329,7 +20322,7 @@
         <v>1.686E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>-9.5189999999999997E-3</v>
       </c>
@@ -20433,7 +20426,7 @@
         <v>1.614E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>-9.5060000000000006E-3</v>
       </c>
@@ -20537,7 +20530,7 @@
         <v>1.4649999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>-9.6299999999999997E-3</v>
       </c>
@@ -20641,7 +20634,7 @@
         <v>1.3699999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>-9.3120000000000008E-3</v>
       </c>
@@ -20745,7 +20738,7 @@
         <v>1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>-9.6340000000000002E-3</v>
       </c>
@@ -20849,7 +20842,7 @@
         <v>1.4059999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>-9.502E-3</v>
       </c>
@@ -20953,7 +20946,7 @@
         <v>1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>-9.3539999999999995E-3</v>
       </c>
@@ -21057,7 +21050,7 @@
         <v>1.4909999999999999E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>-9.4149999999999998E-3</v>
       </c>
@@ -21161,7 +21154,7 @@
         <v>1.485E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>-9.0530000000000003E-3</v>
       </c>
@@ -21265,7 +21258,7 @@
         <v>1.5479999999999999E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>-8.7790000000000003E-3</v>
       </c>
@@ -21369,7 +21362,7 @@
         <v>1.5139999999999999E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>-8.6960000000000006E-3</v>
       </c>
@@ -21473,7 +21466,7 @@
         <v>1.4729999999999999E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>-8.8369999999999994E-3</v>
       </c>
@@ -21577,7 +21570,7 @@
         <v>1.6180000000000001E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>-2.0132000000000001E-2</v>
       </c>
@@ -21683,10 +21676,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'master' into master"
This reverts commit e63157b8daff47e63cb12aa194e32a451b1a39a9, reversing
changes made to e14547ed0b76f38013a3e59f0680a7fcc1b84566.
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00002.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_CE01ISSP_00002.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgarzio/Documents/repo/lgarzio/ooi-integration-fork/asset-management/ARCHIVE/deployment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CE_mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="11420" windowWidth="25600" windowHeight="16060" tabRatio="579" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="579"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -26,11 +26,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$I$51</definedName>
     <definedName name="Workbook1" localSheetId="1">Asset_Cal_Info!$H$5:$H$5</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -51,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="113">
   <si>
     <t>Ref Des</t>
   </si>
@@ -403,9 +400,6 @@
   </si>
   <si>
     <t>Sensor OOIBARCODE</t>
-  </si>
-  <si>
-    <t>corrected cal values: [0.00283856, 0.000119430, 2.41799e-06, 231.190, -0.328248, -55.9998, 4.55859]</t>
   </si>
 </sst>
 </file>
@@ -2252,28 +2246,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2311,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -2355,13 +2349,13 @@
         <v>-124.09566666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
@@ -2370,7 +2364,7 @@
         <v>44.664153333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -2379,73 +2373,73 @@
         <v>-124.09566666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:14" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="4:7" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:7" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
@@ -2454,33 +2448,38 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="5" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="17" style="47" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" customWidth="1"/>
-    <col min="8" max="8" width="37.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" customWidth="1"/>
+    <col min="8" max="8" width="37.44140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2509,7 +2508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -2520,7 +2519,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>104</v>
       </c>
       <c r="F3" s="44">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>7</v>
@@ -2549,7 +2548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>91</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>104</v>
       </c>
       <c r="F4" s="44">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>8</v>
@@ -2578,7 +2577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>91</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>104</v>
       </c>
       <c r="F5" s="44">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>6</v>
@@ -2603,9 +2602,7 @@
       <c r="H5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>113</v>
-      </c>
+      <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -2613,7 +2610,7 @@
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
     </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>91</v>
       </c>
@@ -2630,7 +2627,7 @@
         <v>104</v>
       </c>
       <c r="F6" s="44">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>62</v>
@@ -2642,7 +2639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="21"/>
@@ -2653,7 +2650,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>92</v>
       </c>
@@ -2682,7 +2679,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>92</v>
       </c>
@@ -2709,7 +2706,7 @@
       </c>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>92</v>
       </c>
@@ -2736,7 +2733,7 @@
       </c>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>92</v>
       </c>
@@ -2763,7 +2760,7 @@
       </c>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>92</v>
       </c>
@@ -2790,7 +2787,7 @@
       </c>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>92</v>
       </c>
@@ -2817,7 +2814,7 @@
       </c>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>92</v>
       </c>
@@ -2844,7 +2841,7 @@
       </c>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>92</v>
       </c>
@@ -2871,7 +2868,7 @@
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="21"/>
@@ -2882,7 +2879,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>93</v>
       </c>
@@ -2911,7 +2908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>93</v>
       </c>
@@ -2940,7 +2937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="21"/>
@@ -2951,7 +2948,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>94</v>
       </c>
@@ -2980,7 +2977,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>94</v>
       </c>
@@ -3009,7 +3006,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>94</v>
       </c>
@@ -3038,7 +3035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>94</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>94</v>
       </c>
@@ -3096,7 +3093,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>94</v>
       </c>
@@ -3125,7 +3122,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>94</v>
       </c>
@@ -3154,7 +3151,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="21"/>
@@ -3165,7 +3162,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>95</v>
       </c>
@@ -3192,7 +3189,7 @@
       </c>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>95</v>
       </c>
@@ -3219,7 +3216,7 @@
       </c>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>95</v>
       </c>
@@ -3246,7 +3243,7 @@
       </c>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="21"/>
@@ -3257,7 +3254,7 @@
       <c r="H31" s="19"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>96</v>
       </c>
@@ -3286,7 +3283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>96</v>
       </c>
@@ -3315,7 +3312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>96</v>
       </c>
@@ -3344,7 +3341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>96</v>
       </c>
@@ -3373,7 +3370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>96</v>
       </c>
@@ -3402,7 +3399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>96</v>
       </c>
@@ -3431,7 +3428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>96</v>
       </c>
@@ -3460,7 +3457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>96</v>
       </c>
@@ -3489,7 +3486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>96</v>
       </c>
@@ -3518,7 +3515,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>96</v>
       </c>
@@ -3547,7 +3544,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="21"/>
@@ -3558,7 +3555,7 @@
       <c r="H42" s="19"/>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>97</v>
       </c>
@@ -3587,7 +3584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
         <v>97</v>
       </c>
@@ -3616,7 +3613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="21"/>
@@ -3627,7 +3624,7 @@
       <c r="H45" s="19"/>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
         <v>98</v>
       </c>
@@ -3654,7 +3651,7 @@
       </c>
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>98</v>
       </c>
@@ -3681,7 +3678,7 @@
       </c>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
         <v>98</v>
       </c>
@@ -3708,7 +3705,7 @@
       </c>
       <c r="I48" s="14"/>
     </row>
-    <row r="49" spans="1:9" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" s="9" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
@@ -3719,7 +3716,7 @@
       <c r="H49" s="28"/>
       <c r="I49" s="27"/>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29" t="s">
         <v>99</v>
       </c>
@@ -3742,22 +3739,27 @@
       <c r="H50" s="30"/>
       <c r="I50" s="14"/>
     </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F51" s="47"/>
     </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F52" s="47"/>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F53" s="47"/>
     </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F54" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="3" scale="89" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3769,9 +3771,9 @@
       <selection sqref="A1:AH86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>-2.7306E-2</v>
       </c>
@@ -3875,7 +3877,7 @@
         <v>2.2003000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-2.1257999999999999E-2</v>
       </c>
@@ -3979,7 +3981,7 @@
         <v>1.6747000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-1.2599000000000001E-2</v>
       </c>
@@ -4083,7 +4085,7 @@
         <v>1.111E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-4.3949999999999996E-3</v>
       </c>
@@ -4187,7 +4189,7 @@
         <v>3.9740000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2.9880000000000002E-3</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>-3.1E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7.7140000000000004E-3</v>
       </c>
@@ -4395,7 +4397,7 @@
         <v>-3.039E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1.038E-2</v>
       </c>
@@ -4499,7 +4501,7 @@
         <v>-4.8900000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.0441000000000001E-2</v>
       </c>
@@ -4603,7 +4605,7 @@
         <v>-5.3030000000000004E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9.8150000000000008E-3</v>
       </c>
@@ -4707,7 +4709,7 @@
         <v>-5.378E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9.7280000000000005E-3</v>
       </c>
@@ -4811,7 +4813,7 @@
         <v>-5.0800000000000003E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9.1170000000000001E-3</v>
       </c>
@@ -4915,7 +4917,7 @@
         <v>-5.104E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9.0360000000000006E-3</v>
       </c>
@@ -5019,7 +5021,7 @@
         <v>-4.7270000000000003E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8.0409999999999995E-3</v>
       </c>
@@ -5123,7 +5125,7 @@
         <v>-4.3819999999999996E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8.1829999999999993E-3</v>
       </c>
@@ -5227,7 +5229,7 @@
         <v>-4.5630000000000002E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8.2159999999999993E-3</v>
       </c>
@@ -5331,7 +5333,7 @@
         <v>-4.4270000000000004E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7.6169999999999996E-3</v>
       </c>
@@ -5435,7 +5437,7 @@
         <v>-4.1739999999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6.7520000000000002E-3</v>
       </c>
@@ -5539,7 +5541,7 @@
         <v>-4.1269999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7.0699999999999999E-3</v>
       </c>
@@ -5643,7 +5645,7 @@
         <v>-4.1380000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6.8310000000000003E-3</v>
       </c>
@@ -5747,7 +5749,7 @@
         <v>-4.1419999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6.4079999999999996E-3</v>
       </c>
@@ -5851,7 +5853,7 @@
         <v>-4.2430000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>6.4419999999999998E-3</v>
       </c>
@@ -5955,7 +5957,7 @@
         <v>-4.2009999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6.2509999999999996E-3</v>
       </c>
@@ -6059,7 +6061,7 @@
         <v>-4.0699999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6.1939999999999999E-3</v>
       </c>
@@ -6163,7 +6165,7 @@
         <v>-3.9050000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5.6759999999999996E-3</v>
       </c>
@@ -6267,7 +6269,7 @@
         <v>-3.9870000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5.3439999999999998E-3</v>
       </c>
@@ -6371,7 +6373,7 @@
         <v>-3.7260000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5.2090000000000001E-3</v>
       </c>
@@ -6475,7 +6477,7 @@
         <v>-3.5729999999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4.9170000000000004E-3</v>
       </c>
@@ -6579,7 +6581,7 @@
         <v>-3.578E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4.7239999999999999E-3</v>
       </c>
@@ -6683,7 +6685,7 @@
         <v>-3.392E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4.0660000000000002E-3</v>
       </c>
@@ -6787,7 +6789,7 @@
         <v>-3.2490000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4.2430000000000002E-3</v>
       </c>
@@ -6891,7 +6893,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3.777E-3</v>
       </c>
@@ -6995,7 +6997,7 @@
         <v>-3.0130000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3.607E-3</v>
       </c>
@@ -7099,7 +7101,7 @@
         <v>-2.7659999999999998E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3.2729999999999999E-3</v>
       </c>
@@ -7203,7 +7205,7 @@
         <v>-2.5219999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3.0950000000000001E-3</v>
       </c>
@@ -7307,7 +7309,7 @@
         <v>-2.2269999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3.0699999999999998E-3</v>
       </c>
@@ -7411,7 +7413,7 @@
         <v>-1.8309999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3.0349999999999999E-3</v>
       </c>
@@ -7515,7 +7517,7 @@
         <v>-1.588E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3.2399999999999998E-3</v>
       </c>
@@ -7619,7 +7621,7 @@
         <v>-1.4289999999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3.1510000000000002E-3</v>
       </c>
@@ -7723,7 +7725,7 @@
         <v>-1.129E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3.0019999999999999E-3</v>
       </c>
@@ -7827,7 +7829,7 @@
         <v>-1.0009999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2.911E-3</v>
       </c>
@@ -7931,7 +7933,7 @@
         <v>-9.6299999999999999E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2.9169999999999999E-3</v>
       </c>
@@ -8035,7 +8037,7 @@
         <v>-9.0200000000000002E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2.4870000000000001E-3</v>
       </c>
@@ -8139,7 +8141,7 @@
         <v>-8.8800000000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2.565E-3</v>
       </c>
@@ -8243,7 +8245,7 @@
         <v>-8.7500000000000002E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2.1519999999999998E-3</v>
       </c>
@@ -8347,7 +8349,7 @@
         <v>-9.0399999999999996E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1.918E-3</v>
       </c>
@@ -8451,7 +8453,7 @@
         <v>1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2.2130000000000001E-3</v>
       </c>
@@ -8555,7 +8557,7 @@
         <v>1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2.3509999999999998E-3</v>
       </c>
@@ -8659,7 +8661,7 @@
         <v>-8.2999999999999998E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2.6870000000000002E-3</v>
       </c>
@@ -8763,7 +8765,7 @@
         <v>-1.3200000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2.7929999999999999E-3</v>
       </c>
@@ -8867,7 +8869,7 @@
         <v>-3.5399999999999999E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2.7260000000000001E-3</v>
       </c>
@@ -8971,7 +8973,7 @@
         <v>-4.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2.859E-3</v>
       </c>
@@ -9075,7 +9077,7 @@
         <v>-4.6200000000000001E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2.8110000000000001E-3</v>
       </c>
@@ -9179,7 +9181,7 @@
         <v>-6.5300000000000004E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2.5959999999999998E-3</v>
       </c>
@@ -9283,7 +9285,7 @@
         <v>-6.4199999999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2.3879999999999999E-3</v>
       </c>
@@ -9387,7 +9389,7 @@
         <v>-6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2.1250000000000002E-3</v>
       </c>
@@ -9491,7 +9493,7 @@
         <v>-7.5299999999999998E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1.838E-3</v>
       </c>
@@ -9595,7 +9597,7 @@
         <v>-7.6499999999999995E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1.5709999999999999E-3</v>
       </c>
@@ -9699,7 +9701,7 @@
         <v>-8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1.358E-3</v>
       </c>
@@ -9803,7 +9805,7 @@
         <v>-8.6399999999999997E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1.088E-3</v>
       </c>
@@ -9907,7 +9909,7 @@
         <v>-9.5699999999999995E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>8.8999999999999995E-4</v>
       </c>
@@ -10011,7 +10013,7 @@
         <v>-9.4300000000000004E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4.75E-4</v>
       </c>
@@ -10115,7 +10117,7 @@
         <v>-1.0709999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2.5300000000000002E-4</v>
       </c>
@@ -10219,7 +10221,7 @@
         <v>-1.163E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2.23E-4</v>
       </c>
@@ -10323,7 +10325,7 @@
         <v>-1.232E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>-2.13E-4</v>
       </c>
@@ -10427,7 +10429,7 @@
         <v>-1.2899999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>-3.5300000000000002E-4</v>
       </c>
@@ -10531,7 +10533,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>-6.9099999999999999E-4</v>
       </c>
@@ -10635,7 +10637,7 @@
         <v>-1.371E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>-6.6200000000000005E-4</v>
       </c>
@@ -10739,7 +10741,7 @@
         <v>-1.4250000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>-8.6600000000000002E-4</v>
       </c>
@@ -10843,7 +10845,7 @@
         <v>-1.436E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>-9.8299999999999993E-4</v>
       </c>
@@ -10947,7 +10949,7 @@
         <v>-1.5219999999999999E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>-1.134E-3</v>
       </c>
@@ -11051,7 +11053,7 @@
         <v>-1.578E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>-1.106E-3</v>
       </c>
@@ -11155,7 +11157,7 @@
         <v>-1.518E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>-1.542E-3</v>
       </c>
@@ -11259,7 +11261,7 @@
         <v>-1.5120000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>-1.658E-3</v>
       </c>
@@ -11363,7 +11365,7 @@
         <v>-1.4729999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>-1.7930000000000001E-3</v>
       </c>
@@ -11467,7 +11469,7 @@
         <v>-1.3110000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>-1.9610000000000001E-3</v>
       </c>
@@ -11571,7 +11573,7 @@
         <v>-1.0709999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>-1.92E-3</v>
       </c>
@@ -11675,7 +11677,7 @@
         <v>-8.12E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>-2.1649999999999998E-3</v>
       </c>
@@ -11779,7 +11781,7 @@
         <v>-5.9800000000000001E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>-2.274E-3</v>
       </c>
@@ -11883,7 +11885,7 @@
         <v>-3.3300000000000002E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>-2.4229999999999998E-3</v>
       </c>
@@ -11987,7 +11989,7 @@
         <v>-2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>-2.5240000000000002E-3</v>
       </c>
@@ -12091,7 +12093,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>-2.5490000000000001E-3</v>
       </c>
@@ -12195,7 +12197,7 @@
         <v>2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>-2.5799999999999998E-3</v>
       </c>
@@ -12299,7 +12301,7 @@
         <v>4.5600000000000003E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>-2.421E-3</v>
       </c>
@@ -12403,7 +12405,7 @@
         <v>4.3100000000000001E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>-2.4420000000000002E-3</v>
       </c>
@@ -12507,7 +12509,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>-2.117E-3</v>
       </c>
@@ -12611,7 +12613,7 @@
         <v>4.8200000000000001E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>-2.3029999999999999E-3</v>
       </c>
@@ -12717,6 +12719,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12728,9 +12735,9 @@
       <selection sqref="A1:AH86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>2.818E-2</v>
       </c>
@@ -12834,7 +12841,7 @@
         <v>-1.3003000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.9113999999999999E-2</v>
       </c>
@@ -12938,7 +12945,7 @@
         <v>-1.0573000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.0387E-2</v>
       </c>
@@ -13042,7 +13049,7 @@
         <v>-9.0050000000000009E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6.8069999999999997E-3</v>
       </c>
@@ -13146,7 +13153,7 @@
         <v>-8.1989999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5.4920000000000004E-3</v>
       </c>
@@ -13250,7 +13257,7 @@
         <v>-6.4209999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.483E-3</v>
       </c>
@@ -13354,7 +13361,7 @@
         <v>-5.2810000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2.4060000000000002E-3</v>
       </c>
@@ -13458,7 +13465,7 @@
         <v>-4.2729999999999999E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1.4300000000000001E-3</v>
       </c>
@@ -13562,7 +13569,7 @@
         <v>-3.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-1.129E-3</v>
       </c>
@@ -13666,7 +13673,7 @@
         <v>-2.5100000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-1.812E-3</v>
       </c>
@@ -13770,7 +13777,7 @@
         <v>-1.8680000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-2.7070000000000002E-3</v>
       </c>
@@ -13874,7 +13881,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>-4.6169999999999996E-3</v>
       </c>
@@ -13978,7 +13985,7 @@
         <v>-7.1100000000000004E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-4.8739999999999999E-3</v>
       </c>
@@ -14082,7 +14089,7 @@
         <v>-5.8999999999999998E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>-5.3109999999999997E-3</v>
       </c>
@@ -14186,7 +14193,7 @@
         <v>6.6600000000000003E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>-6.7479999999999997E-3</v>
       </c>
@@ -14290,7 +14297,7 @@
         <v>9.2900000000000003E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-6.149E-3</v>
       </c>
@@ -14394,7 +14401,7 @@
         <v>1.4610000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-6.437E-3</v>
       </c>
@@ -14498,7 +14505,7 @@
         <v>1.7589999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-7.2789999999999999E-3</v>
       </c>
@@ -14602,7 +14609,7 @@
         <v>2.1549999999999998E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>-7.6649999999999999E-3</v>
       </c>
@@ -14706,7 +14713,7 @@
         <v>2.1870000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-8.8280000000000008E-3</v>
       </c>
@@ -14810,7 +14817,7 @@
         <v>2.5990000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-9.3799999999999994E-3</v>
       </c>
@@ -14914,7 +14921,7 @@
         <v>2.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-9.2580000000000006E-3</v>
       </c>
@@ -15018,7 +15025,7 @@
         <v>2.8349999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>-1.0026E-2</v>
       </c>
@@ -15122,7 +15129,7 @@
         <v>2.7989999999999998E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-1.0159E-2</v>
       </c>
@@ -15226,7 +15233,7 @@
         <v>2.8739999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>-9.9780000000000008E-3</v>
       </c>
@@ -15330,7 +15337,7 @@
         <v>2.8479999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>-1.0371E-2</v>
       </c>
@@ -15434,7 +15441,7 @@
         <v>2.7680000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>-1.0656000000000001E-2</v>
       </c>
@@ -15538,7 +15545,7 @@
         <v>2.8119999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>-1.0642E-2</v>
       </c>
@@ -15642,7 +15649,7 @@
         <v>2.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>-1.0969E-2</v>
       </c>
@@ -15746,7 +15753,7 @@
         <v>2.7669999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>-1.1292E-2</v>
       </c>
@@ -15850,7 +15857,7 @@
         <v>2.771E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>-1.0963000000000001E-2</v>
       </c>
@@ -15954,7 +15961,7 @@
         <v>2.5690000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>-1.1731999999999999E-2</v>
       </c>
@@ -16058,7 +16065,7 @@
         <v>2.506E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>-1.1818E-2</v>
       </c>
@@ -16162,7 +16169,7 @@
         <v>2.369E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>-1.2111E-2</v>
       </c>
@@ -16266,7 +16273,7 @@
         <v>2.212E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>-1.2655E-2</v>
       </c>
@@ -16370,7 +16377,7 @@
         <v>2.1180000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>-1.2838E-2</v>
       </c>
@@ -16474,7 +16481,7 @@
         <v>2.0839999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>-1.2978999999999999E-2</v>
       </c>
@@ -16578,7 +16585,7 @@
         <v>2.0790000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>-1.304E-2</v>
       </c>
@@ -16682,7 +16689,7 @@
         <v>2.0609999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>-1.2704999999999999E-2</v>
       </c>
@@ -16786,7 +16793,7 @@
         <v>2.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>-1.2663000000000001E-2</v>
       </c>
@@ -16890,7 +16897,7 @@
         <v>2.0089999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>-1.2364999999999999E-2</v>
       </c>
@@ -16994,7 +17001,7 @@
         <v>2.032E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>-1.2322E-2</v>
       </c>
@@ -17098,7 +17105,7 @@
         <v>2.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>-1.1955E-2</v>
       </c>
@@ -17202,7 +17209,7 @@
         <v>2.1069999999999999E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>-1.2149E-2</v>
       </c>
@@ -17306,7 +17313,7 @@
         <v>2.0170000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>-7.4850000000000003E-3</v>
       </c>
@@ -17410,7 +17417,7 @@
         <v>8.8599999999999996E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>-7.2389999999999998E-3</v>
       </c>
@@ -17514,7 +17521,7 @@
         <v>7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>-7.123E-3</v>
       </c>
@@ -17618,7 +17625,7 @@
         <v>6.3500000000000004E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>-6.8180000000000003E-3</v>
       </c>
@@ -17722,7 +17729,7 @@
         <v>5.2599999999999999E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>-6.8339999999999998E-3</v>
       </c>
@@ -17826,7 +17833,7 @@
         <v>5.1099999999999995E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>-6.881E-3</v>
       </c>
@@ -17930,7 +17937,7 @@
         <v>6.2399999999999999E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>-6.9410000000000001E-3</v>
       </c>
@@ -18034,7 +18041,7 @@
         <v>6.7599999999999995E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>-7.0809999999999996E-3</v>
       </c>
@@ -18138,7 +18145,7 @@
         <v>8.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>-7.2399999999999999E-3</v>
       </c>
@@ -18242,7 +18249,7 @@
         <v>9.2699999999999998E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>-7.4229999999999999E-3</v>
       </c>
@@ -18346,7 +18353,7 @@
         <v>1.114E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>-7.6220000000000003E-3</v>
       </c>
@@ -18450,7 +18457,7 @@
         <v>1.3140000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>-7.8150000000000008E-3</v>
       </c>
@@ -18554,7 +18561,7 @@
         <v>1.4549999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>-8.0059999999999992E-3</v>
       </c>
@@ -18658,7 +18665,7 @@
         <v>1.5709999999999999E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>-8.1650000000000004E-3</v>
       </c>
@@ -18762,7 +18769,7 @@
         <v>1.604E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>-8.2880000000000002E-3</v>
       </c>
@@ -18866,7 +18873,7 @@
         <v>1.784E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>-8.456E-3</v>
       </c>
@@ -18970,7 +18977,7 @@
         <v>1.8600000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>-8.6499999999999997E-3</v>
       </c>
@@ -19074,7 +19081,7 @@
         <v>1.897E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>-8.6359999999999996E-3</v>
       </c>
@@ -19178,7 +19185,7 @@
         <v>1.7960000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>-8.2819999999999994E-3</v>
       </c>
@@ -19282,7 +19289,7 @@
         <v>1.9239999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>-8.7810000000000006E-3</v>
       </c>
@@ -19386,7 +19393,7 @@
         <v>1.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>-8.659E-3</v>
       </c>
@@ -19490,7 +19497,7 @@
         <v>1.9350000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>-8.5939999999999992E-3</v>
       </c>
@@ -19594,7 +19601,7 @@
         <v>1.9689999999999998E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>-8.9849999999999999E-3</v>
       </c>
@@ -19698,7 +19705,7 @@
         <v>1.884E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>-8.744E-3</v>
       </c>
@@ -19802,7 +19809,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>-8.9210000000000001E-3</v>
       </c>
@@ -19906,7 +19913,7 @@
         <v>1.913E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>-8.9890000000000005E-3</v>
       </c>
@@ -20010,7 +20017,7 @@
         <v>1.8760000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>-9.1999999999999998E-3</v>
       </c>
@@ -20114,7 +20121,7 @@
         <v>1.8259999999999999E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>-9.391E-3</v>
       </c>
@@ -20218,7 +20225,7 @@
         <v>1.7700000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>-9.4769999999999993E-3</v>
       </c>
@@ -20322,7 +20329,7 @@
         <v>1.686E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>-9.5189999999999997E-3</v>
       </c>
@@ -20426,7 +20433,7 @@
         <v>1.614E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>-9.5060000000000006E-3</v>
       </c>
@@ -20530,7 +20537,7 @@
         <v>1.4649999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>-9.6299999999999997E-3</v>
       </c>
@@ -20634,7 +20641,7 @@
         <v>1.3699999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>-9.3120000000000008E-3</v>
       </c>
@@ -20738,7 +20745,7 @@
         <v>1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>-9.6340000000000002E-3</v>
       </c>
@@ -20842,7 +20849,7 @@
         <v>1.4059999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>-9.502E-3</v>
       </c>
@@ -20946,7 +20953,7 @@
         <v>1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>-9.3539999999999995E-3</v>
       </c>
@@ -21050,7 +21057,7 @@
         <v>1.4909999999999999E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>-9.4149999999999998E-3</v>
       </c>
@@ -21154,7 +21161,7 @@
         <v>1.485E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>-9.0530000000000003E-3</v>
       </c>
@@ -21258,7 +21265,7 @@
         <v>1.5479999999999999E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>-8.7790000000000003E-3</v>
       </c>
@@ -21362,7 +21369,7 @@
         <v>1.5139999999999999E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>-8.6960000000000006E-3</v>
       </c>
@@ -21466,7 +21473,7 @@
         <v>1.4729999999999999E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>-8.8369999999999994E-3</v>
       </c>
@@ -21570,7 +21577,7 @@
         <v>1.6180000000000001E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>-2.0132000000000001E-2</v>
       </c>
@@ -21676,5 +21683,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>